<commit_message>
fix getting N issue, add database backup and restore functions
</commit_message>
<xml_diff>
--- a/server/corelib/lang/all_lang_V2.0.xlsx
+++ b/server/corelib/lang/all_lang_V2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digiCenter\server\corelib\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD6FE21-CAB6-47A4-B5C2-B8AD33E6E681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3A06A9-51ED-42D9-828F-D562AAA8CD5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18120" yWindow="-1770" windowWidth="18240" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="1268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="1313">
   <si>
     <t>name</t>
   </si>
@@ -4244,6 +4244,168 @@
   </si>
   <si>
     <t>请点击继续按钮以继续测试</t>
+  </si>
+  <si>
+    <t>server_database_backup_ok</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>server_database_backup_NG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Database Backup and Restore</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>db_backup_restore_title</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>backup_db_btn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>restore_db_btn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backup</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Restore</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Database backup successfully!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Database backup failed!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>server_database_restore_ok</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>server_database_restore_NG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Database restore successfully!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Database restore failed!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>資料庫備份成功</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>資料庫備份失敗</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>資料庫備份與還原</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>備份</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>還原</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>資料庫還原成功</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>資料庫還原失敗</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Datenbank-Backup erfolgreich!</t>
+  </si>
+  <si>
+    <t>资料库备份成功</t>
+  </si>
+  <si>
+    <t>Datenbanksicherung fehlgeschlagen!</t>
+  </si>
+  <si>
+    <t>资料库备份失败</t>
+  </si>
+  <si>
+    <t>Datenbank-Backup und Wiederherstellung</t>
+  </si>
+  <si>
+    <t>资料库备份与还原</t>
+  </si>
+  <si>
+    <t>Sicherungskopie</t>
+  </si>
+  <si>
+    <t>备份</t>
+  </si>
+  <si>
+    <t>Wiederherstellen</t>
+  </si>
+  <si>
+    <t>还原</t>
+  </si>
+  <si>
+    <t>Datenbank wiederherstellen erfolgreich!</t>
+  </si>
+  <si>
+    <t>资料库还原成功</t>
+  </si>
+  <si>
+    <t>Datenbank Wiederherstellung fehlgeschlagen!</t>
+  </si>
+  <si>
+    <t>资料库还原失败</t>
+  </si>
+  <si>
+    <t>side_database</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>備份與還原</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backup and Restore</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sichern und Wiederherstellen</t>
+  </si>
+  <si>
+    <t>备份与还原</t>
+  </si>
+  <si>
+    <t>server_restart_program</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Please restart the program!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>請重新開啟程式</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bitte starten Sie das Programm!</t>
+  </si>
+  <si>
+    <t>请重新开启程式</t>
   </si>
 </sst>
 </file>
@@ -4395,7 +4557,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="78">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5490,10 +5672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F276"/>
+  <dimension ref="A1:F285"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A250" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B275" sqref="B275"/>
+      <selection activeCell="B285" sqref="B285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11021,384 +11203,574 @@
         <v>1267</v>
       </c>
     </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277" s="2">
+        <v>276</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>1282</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F277" s="1" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278" s="2">
+        <v>277</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F278" s="1" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" s="2">
+        <v>278</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>1293</v>
+      </c>
+      <c r="F279" s="1" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" s="2">
+        <v>279</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F280" s="1" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" s="2">
+        <v>280</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>1297</v>
+      </c>
+      <c r="F281" s="1" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282" s="2">
+        <v>281</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="F282" s="1" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283" s="2">
+        <v>282</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F283" s="1" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284" s="2">
+        <v>283</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="F284" s="1" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285" s="2">
+        <v>284</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="F285" s="1" t="s">
+        <v>1312</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B168:E169 B1:E3 B154:E155 B97:E152 B69:E72 B5:E6 B17:E29 B179:E194 B211:D211 B217:E218 B75:E84 B257:E257 D253:E253 C243:E248 B259:C259 B8:E14 B7:D7 B15:D15 B31:E38 B30:D30 B40:E46 B39:D39 B48:E61 B47:D47 B86:E88 B85:D85 B157:E159 B156:D156 B161:E161 B160:D160 B164:E166 B162:D163 B202:E205 B207:E207 B206:D206 B214:D216 B220:E220 B219:D219 B222:E222 B221:D221 B224:E225 B223:D223 B227:E230 B226:D226 B233:E233 B231:D232 B235:E235 B234:D234 B237:E239 B236:D236 C242:D242 C250:E250 C249:D249 D252 D256:E256 D254:D255 B260 B261:E266 B89:D89 B196:E199 B195:D195 B200:D201 B241:E241 B240:D240 B258:D258 B272:E273 B63:E66 B62:C62 C251 B275:E1048576">
+  <conditionalFormatting sqref="B168:E169 B1:E3 B154:E155 B97:E152 B69:E72 B5:E6 B17:E29 B179:E194 B211:D211 B217:E218 B75:E84 B257:E257 D253:E253 C243:E248 B259:C259 B8:E14 B7:D7 B15:D15 B31:E38 B30:D30 B40:E46 B39:D39 B48:E61 B47:D47 B86:E88 B85:D85 B157:E159 B156:D156 B161:E161 B160:D160 B164:E166 B162:D163 B202:E205 B207:E207 B206:D206 B214:D216 B220:E220 B219:D219 B222:E222 B221:D221 B224:E225 B223:D223 B227:E230 B226:D226 B233:E233 B231:D232 B235:E235 B234:D234 B237:E239 B236:D236 C242:D242 C250:E250 C249:D249 D252 D256:E256 D254:D255 B260 B261:E266 B89:D89 B196:E199 B195:D195 B200:D201 B241:E241 B240:D240 B258:D258 B272:E273 B63:E66 B62:C62 C251 B275:E281 B284:E1048576">
+    <cfRule type="cellIs" dxfId="77" priority="81" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B167:E167">
+    <cfRule type="cellIs" dxfId="76" priority="80" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B171:E172">
     <cfRule type="cellIs" dxfId="75" priority="79" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B167:E167">
+  <conditionalFormatting sqref="B153:D153">
     <cfRule type="cellIs" dxfId="74" priority="78" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B171:E172">
+  <conditionalFormatting sqref="B173:D173 B174 D174:E174">
     <cfRule type="cellIs" dxfId="73" priority="77" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B153:D153">
+  <conditionalFormatting sqref="B175:E175 B176 D176">
     <cfRule type="cellIs" dxfId="72" priority="76" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B173:D173 B174 D174:E174">
+  <conditionalFormatting sqref="B177:E177 B178:D178">
     <cfRule type="cellIs" dxfId="71" priority="75" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B175:E175 B176 D176">
+  <conditionalFormatting sqref="C176">
     <cfRule type="cellIs" dxfId="70" priority="74" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B177:E177 B178:D178">
+  <conditionalFormatting sqref="C174">
     <cfRule type="cellIs" dxfId="69" priority="73" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C176">
+  <conditionalFormatting sqref="B90:E90">
     <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C174">
+  <conditionalFormatting sqref="B91:D93">
     <cfRule type="cellIs" dxfId="67" priority="71" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B90:E90">
+  <conditionalFormatting sqref="E91:E92">
     <cfRule type="cellIs" dxfId="66" priority="70" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B91:D93">
+  <conditionalFormatting sqref="B94:D94 B96:D96">
     <cfRule type="cellIs" dxfId="65" priority="69" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E91:E92">
+  <conditionalFormatting sqref="E96">
     <cfRule type="cellIs" dxfId="64" priority="68" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B94:D94 B96:D96">
+  <conditionalFormatting sqref="B4:E4">
     <cfRule type="cellIs" dxfId="63" priority="67" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E96">
+  <conditionalFormatting sqref="B67:E68">
     <cfRule type="cellIs" dxfId="62" priority="66" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4">
+  <conditionalFormatting sqref="B208:E209">
     <cfRule type="cellIs" dxfId="61" priority="65" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67:E68">
+  <conditionalFormatting sqref="B73:D74">
     <cfRule type="cellIs" dxfId="60" priority="64" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B208:E209">
+  <conditionalFormatting sqref="E74">
     <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B73:D74">
+  <conditionalFormatting sqref="E73">
     <cfRule type="cellIs" dxfId="58" priority="62" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
+  <conditionalFormatting sqref="B16:D16">
     <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
+  <conditionalFormatting sqref="E93">
     <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:D16">
+  <conditionalFormatting sqref="B207:E207">
     <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E93">
+  <conditionalFormatting sqref="B206:D206">
     <cfRule type="cellIs" dxfId="54" priority="58" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B207:E207">
+  <conditionalFormatting sqref="F168:F169 F1:F3 F154:F166 F97:F152 F69:F72 F5:F15 F75:F89 F17:F61 F179:F207 F211 F214:F250 F261:F266 F272:F273 F63:F66 F252:F258 F275:F281 F284:F1048576">
     <cfRule type="cellIs" dxfId="53" priority="57" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B206:D206">
+  <conditionalFormatting sqref="F167">
     <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F168:F169 F1:F3 F154:F166 F97:F152 F69:F72 F5:F15 F75:F89 F17:F61 F179:F207 F211 F214:F250 F261:F266 F272:F273 F63:F66 F252:F258 F275:F1048576">
+  <conditionalFormatting sqref="F171:F172">
     <cfRule type="cellIs" dxfId="51" priority="55" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F167">
+  <conditionalFormatting sqref="F153">
     <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F171:F172">
+  <conditionalFormatting sqref="F173:F174">
     <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F153">
+  <conditionalFormatting sqref="F175:F176">
     <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F173:F174">
+  <conditionalFormatting sqref="F177:F178">
     <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F175:F176">
+  <conditionalFormatting sqref="F90">
     <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F177:F178">
+  <conditionalFormatting sqref="F91:F93">
     <cfRule type="cellIs" dxfId="45" priority="49" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90">
+  <conditionalFormatting sqref="F94 F96">
     <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F91:F93">
+  <conditionalFormatting sqref="F4">
     <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F94 F96">
+  <conditionalFormatting sqref="F67:F68">
     <cfRule type="cellIs" dxfId="42" priority="46" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
+  <conditionalFormatting sqref="F208:F209">
     <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F67:F68">
+  <conditionalFormatting sqref="F73:F74">
     <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F208:F209">
+  <conditionalFormatting sqref="F16">
     <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F73:F74">
+  <conditionalFormatting sqref="F207">
     <cfRule type="cellIs" dxfId="38" priority="42" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
+  <conditionalFormatting sqref="F206">
     <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F207">
-    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F206">
-    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B212:E212">
-    <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F212">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B210:E210">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F210">
     <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B210:E210">
+  <conditionalFormatting sqref="B170:D170">
     <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F210">
+  <conditionalFormatting sqref="F170">
     <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B170:D170">
+  <conditionalFormatting sqref="B95:D95">
     <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F170">
+  <conditionalFormatting sqref="E95">
     <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B95:D95">
+  <conditionalFormatting sqref="F95">
     <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E95">
+  <conditionalFormatting sqref="B213:D213">
     <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F95">
+  <conditionalFormatting sqref="F213">
     <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B213:D213">
+  <conditionalFormatting sqref="C252:C256">
     <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F213">
+  <conditionalFormatting sqref="B242:B251">
     <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C252:C256">
+  <conditionalFormatting sqref="B252:B256">
     <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B242:B251">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+  <conditionalFormatting sqref="D259">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B252:B256">
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+  <conditionalFormatting sqref="F259">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D259">
+  <conditionalFormatting sqref="E153">
     <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F259">
+  <conditionalFormatting sqref="C260 E260">
     <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E153">
+  <conditionalFormatting sqref="D260 F260">
     <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C260 E260">
+  <conditionalFormatting sqref="E160">
     <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D260 F260">
+  <conditionalFormatting sqref="C267:D267">
     <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E160">
+  <conditionalFormatting sqref="F267">
     <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C267:D267">
+  <conditionalFormatting sqref="B267">
     <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F267">
+  <conditionalFormatting sqref="B268:E269">
     <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B267">
+  <conditionalFormatting sqref="F268:F269">
     <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B268:E269">
+  <conditionalFormatting sqref="B270:E270">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F268:F269">
+  <conditionalFormatting sqref="F270">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B270:E270">
+  <conditionalFormatting sqref="B271:E271">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F270">
+  <conditionalFormatting sqref="F271">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B271:E271">
+  <conditionalFormatting sqref="D62:E62">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F271">
+  <conditionalFormatting sqref="F62">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D62:E62">
+  <conditionalFormatting sqref="D251:E251">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F62">
+  <conditionalFormatting sqref="F251">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D251:E251">
+  <conditionalFormatting sqref="B274:E274">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F251">
+  <conditionalFormatting sqref="F274">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B274:E274">
+  <conditionalFormatting sqref="B282:E283">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F274">
+  <conditionalFormatting sqref="F282:F283">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>

</xml_diff>